<commit_message>
merging older docs with new project
</commit_message>
<xml_diff>
--- a/tests/test_data/model/model.xlsx
+++ b/tests/test_data/model/model.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T5"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -526,12 +526,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>/stab/stab.json</t>
+          <t>/model.json</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>12.0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -541,32 +541,32 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>6.0</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>-3.0</t>
+          <t>-6.0</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.125</t>
+          <t>2.25</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-0.375</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>1.5</t>
+          <t>8.0</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>5.84375</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -576,12 +576,12 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>0.0625</t>
+          <t>0.1953125</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>4.501953125</t>
+          <t>59.77620442708333</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -591,7 +591,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>2.490234375</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -601,7 +601,7 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>0.501953125</t>
+          <t>101.23909505208337</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
@@ -611,7 +611,7 @@
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>2.490234375</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
@@ -621,14 +621,14 @@
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>158.47981770833337</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>/body/rudder/rudder.json</t>
+          <t>/stab/stab.json</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -643,47 +643,47 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>3.0</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>-3.0</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>0.125</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>1.5</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
           <t>0.0625</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>-0.0625</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2.0</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>0.5</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>0.16731770833333326</t>
+          <t>4.501953125</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
@@ -703,7 +703,7 @@
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>0.33333333333333326</t>
+          <t>0.501953125</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
@@ -723,14 +723,14 @@
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>0.16731770833333326</t>
+          <t>5.0</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>/body/stick/stick.json</t>
+          <t>/body/body.json</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -755,7 +755,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0.25</t>
+          <t>2.25</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -765,12 +765,12 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>1.5</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>7.25</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -780,12 +780,12 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.3125</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>0.0390625</t>
+          <t>0.7923177083333333</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
@@ -795,7 +795,7 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>-2.34375</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
@@ -805,7 +805,7 @@
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>18.03125</t>
+          <t>28.325520833333314</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
@@ -815,7 +815,7 @@
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>-0.0</t>
+          <t>-2.34375</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
@@ -825,107 +825,311 @@
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>18.0078125</t>
+          <t>27.550130208333314</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>/body/rudder/rudder.json</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2.0</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>0.0625</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>-0.0625</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2.0</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>0.5</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>0.16731770833333326</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>-0.0</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>-0.0</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>-0.0</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>0.33333333333333326</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>-0.0</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>-0.0</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>-0.0</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>0.16731770833333326</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>/body/stick/stick.json</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>12.0</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>0.125</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>-0.125</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>-0.25</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>1.5</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>6.0</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>0.0390625</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>-0.0</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>-0.0</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>-0.0</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>18.03125</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>-0.0</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>-0.0</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>-0.0</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>18.0078125</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>/wing/wing.json</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B7" t="inlineStr">
         <is>
           <t>3.0</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
         <is>
           <t>6.0</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>-6.0</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>0.125</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
         <is>
           <t>4.5</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>1.5</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
         <is>
           <t>0.0625</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
+      <c r="L7" t="inlineStr">
         <is>
           <t>54.005859375</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>-0.0</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>-0.0</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>-0.0</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>-0.0</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>-0.0</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>-0.0</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
         <is>
           <t>3.380859375</t>
         </is>
       </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>-0.0</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>-0.0</t>
-        </is>
-      </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>-0.0</t>
-        </is>
-      </c>
-      <c r="T5" t="inlineStr">
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>-0.0</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>-0.0</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>-0.0</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
         <is>
           <t>57.375</t>
         </is>

</xml_diff>